<commit_message>
Documentei linhas do arquivo Models
</commit_message>
<xml_diff>
--- a/planilha/tarefas.xlsx
+++ b/planilha/tarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="86">
   <si>
     <t>Hoje</t>
   </si>
@@ -52,9 +52,6 @@
     <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
-    <t>27/03/2023  11:42:35</t>
-  </si>
-  <si>
     <t>28/03/2023  12:56:37</t>
   </si>
   <si>
@@ -139,7 +136,10 @@
     <t>11/04/2023  11:09:14</t>
   </si>
   <si>
-    <t>BETHANIA DE PAULA BARBOSA</t>
+    <t>12/04/2023  08:58:03</t>
+  </si>
+  <si>
+    <t>12/04/2023  10:38:24</t>
   </si>
   <si>
     <t>YASMIN SANTOS PALHARES HORTA</t>
@@ -226,7 +226,10 @@
     <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
   </si>
   <si>
-    <t>0 dias úteis</t>
+    <t>LUDIANE CONCEICAO DOS SANTOS OLIVEIRA MATOS</t>
+  </si>
+  <si>
+    <t>ELENICE DE SIQUEIRA</t>
   </si>
   <si>
     <t>1 dias úteis</t>
@@ -257,9 +260,6 @@
   </si>
   <si>
     <t>10 dias úteis</t>
-  </si>
-  <si>
-    <t>SIM</t>
   </si>
   <si>
     <t>NO</t>
@@ -629,7 +629,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -681,19 +681,19 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <v>12142270</v>
+        <v>12144548</v>
       </c>
       <c r="F2">
-        <v>8574731</v>
+        <v>8577545</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s">
         <v>83</v>
@@ -716,16 +716,16 @@
         <v>13</v>
       </c>
       <c r="E3">
-        <v>12144548</v>
+        <v>12144906</v>
       </c>
       <c r="F3">
-        <v>8577545</v>
+        <v>8578064</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
         <v>82</v>
@@ -751,16 +751,16 @@
         <v>14</v>
       </c>
       <c r="E4">
-        <v>12144906</v>
+        <v>12145988</v>
       </c>
       <c r="F4">
-        <v>8578064</v>
+        <v>8579353</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
         <v>82</v>
@@ -786,22 +786,22 @@
         <v>15</v>
       </c>
       <c r="E5">
-        <v>12145988</v>
+        <v>12146576</v>
       </c>
       <c r="F5">
-        <v>8579353</v>
+        <v>8580030</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s">
         <v>82</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s">
         <v>85</v>
@@ -821,16 +821,16 @@
         <v>16</v>
       </c>
       <c r="E6">
-        <v>12146576</v>
+        <v>12146711</v>
       </c>
       <c r="F6">
-        <v>8580030</v>
+        <v>8580119</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s">
         <v>82</v>
@@ -856,16 +856,16 @@
         <v>17</v>
       </c>
       <c r="E7">
-        <v>12146711</v>
+        <v>12146787</v>
       </c>
       <c r="F7">
-        <v>8580119</v>
+        <v>8580243</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I7" t="s">
         <v>82</v>
@@ -891,22 +891,22 @@
         <v>18</v>
       </c>
       <c r="E8">
-        <v>12146787</v>
+        <v>12147152</v>
       </c>
       <c r="F8">
-        <v>8580243</v>
+        <v>8580726</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
         <v>82</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K8" t="s">
         <v>85</v>
@@ -926,16 +926,16 @@
         <v>19</v>
       </c>
       <c r="E9">
-        <v>12147152</v>
+        <v>12147478</v>
       </c>
       <c r="F9">
-        <v>8580726</v>
+        <v>8230607</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I9" t="s">
         <v>82</v>
@@ -961,16 +961,16 @@
         <v>20</v>
       </c>
       <c r="E10">
-        <v>12147478</v>
+        <v>12147631</v>
       </c>
       <c r="F10">
-        <v>8230607</v>
+        <v>8581299</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
         <v>82</v>
@@ -996,16 +996,16 @@
         <v>21</v>
       </c>
       <c r="E11">
-        <v>12147631</v>
+        <v>12148200</v>
       </c>
       <c r="F11">
-        <v>8581299</v>
+        <v>8581975</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
         <v>82</v>
@@ -1031,16 +1031,16 @@
         <v>22</v>
       </c>
       <c r="E12">
-        <v>12148200</v>
+        <v>12149727</v>
       </c>
       <c r="F12">
-        <v>8581975</v>
+        <v>8583861</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I12" t="s">
         <v>82</v>
@@ -1066,22 +1066,22 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>12149727</v>
+        <v>12151325</v>
       </c>
       <c r="F13">
-        <v>8583861</v>
+        <v>8585862</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I13" t="s">
         <v>82</v>
       </c>
       <c r="J13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K13" t="s">
         <v>85</v>
@@ -1101,22 +1101,22 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>12151325</v>
+        <v>12151461</v>
       </c>
       <c r="F14">
-        <v>8585862</v>
+        <v>8586030</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I14" t="s">
         <v>82</v>
       </c>
       <c r="J14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" t="s">
         <v>85</v>
@@ -1136,16 +1136,16 @@
         <v>25</v>
       </c>
       <c r="E15">
-        <v>12151461</v>
+        <v>12153205</v>
       </c>
       <c r="F15">
-        <v>8586030</v>
+        <v>8588077</v>
       </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I15" t="s">
         <v>82</v>
@@ -1171,16 +1171,16 @@
         <v>26</v>
       </c>
       <c r="E16">
-        <v>12153205</v>
+        <v>12153463</v>
       </c>
       <c r="F16">
-        <v>8588077</v>
+        <v>8588431</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
         <v>82</v>
@@ -1206,16 +1206,16 @@
         <v>27</v>
       </c>
       <c r="E17">
-        <v>12153463</v>
+        <v>12153630</v>
       </c>
       <c r="F17">
-        <v>8588431</v>
+        <v>8588645</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
         <v>82</v>
@@ -1241,16 +1241,16 @@
         <v>28</v>
       </c>
       <c r="E18">
-        <v>12153630</v>
+        <v>12154294</v>
       </c>
       <c r="F18">
-        <v>8588645</v>
+        <v>8589407</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I18" t="s">
         <v>82</v>
@@ -1276,16 +1276,16 @@
         <v>29</v>
       </c>
       <c r="E19">
-        <v>12154294</v>
+        <v>12154631</v>
       </c>
       <c r="F19">
-        <v>8589407</v>
+        <v>8589813</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I19" t="s">
         <v>82</v>
@@ -1311,22 +1311,22 @@
         <v>30</v>
       </c>
       <c r="E20">
-        <v>12154631</v>
+        <v>12155655</v>
       </c>
       <c r="F20">
-        <v>8589813</v>
+        <v>8591050</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I20" t="s">
         <v>82</v>
       </c>
       <c r="J20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K20" t="s">
         <v>85</v>
@@ -1346,22 +1346,22 @@
         <v>31</v>
       </c>
       <c r="E21">
-        <v>12155655</v>
+        <v>12155706</v>
       </c>
       <c r="F21">
-        <v>8591050</v>
+        <v>8591067</v>
       </c>
       <c r="G21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I21" t="s">
         <v>82</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K21" t="s">
         <v>85</v>
@@ -1381,16 +1381,16 @@
         <v>32</v>
       </c>
       <c r="E22">
-        <v>12155706</v>
+        <v>12155732</v>
       </c>
       <c r="F22">
-        <v>8591067</v>
+        <v>8591079</v>
       </c>
       <c r="G22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I22" t="s">
         <v>82</v>
@@ -1416,16 +1416,16 @@
         <v>33</v>
       </c>
       <c r="E23">
-        <v>12155732</v>
+        <v>12156130</v>
       </c>
       <c r="F23">
-        <v>8591079</v>
+        <v>8591725</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I23" t="s">
         <v>82</v>
@@ -1451,16 +1451,16 @@
         <v>34</v>
       </c>
       <c r="E24">
-        <v>12156130</v>
+        <v>12157899</v>
       </c>
       <c r="F24">
-        <v>8591725</v>
+        <v>8593801</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I24" t="s">
         <v>82</v>
@@ -1486,16 +1486,16 @@
         <v>35</v>
       </c>
       <c r="E25">
-        <v>12157899</v>
+        <v>12159646</v>
       </c>
       <c r="F25">
-        <v>8593801</v>
+        <v>7797800</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H25" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I25" t="s">
         <v>82</v>
@@ -1521,16 +1521,16 @@
         <v>36</v>
       </c>
       <c r="E26">
-        <v>12159646</v>
+        <v>12161100</v>
       </c>
       <c r="F26">
-        <v>7797800</v>
+        <v>8597675</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I26" t="s">
         <v>82</v>
@@ -1556,16 +1556,16 @@
         <v>37</v>
       </c>
       <c r="E27">
-        <v>12161100</v>
+        <v>12161386</v>
       </c>
       <c r="F27">
-        <v>8597675</v>
+        <v>8598016</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I27" t="s">
         <v>82</v>
@@ -1591,16 +1591,16 @@
         <v>38</v>
       </c>
       <c r="E28">
-        <v>12161386</v>
+        <v>12163407</v>
       </c>
       <c r="F28">
-        <v>8598016</v>
+        <v>8600473</v>
       </c>
       <c r="G28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I28" t="s">
         <v>82</v>
@@ -1626,16 +1626,16 @@
         <v>39</v>
       </c>
       <c r="E29">
-        <v>12163407</v>
+        <v>12163869</v>
       </c>
       <c r="F29">
-        <v>8600473</v>
+        <v>8601052</v>
       </c>
       <c r="G29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I29" t="s">
         <v>82</v>
@@ -1661,16 +1661,16 @@
         <v>40</v>
       </c>
       <c r="E30">
-        <v>12163869</v>
+        <v>12165805</v>
       </c>
       <c r="F30">
-        <v>8601052</v>
+        <v>8603359</v>
       </c>
       <c r="G30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I30" t="s">
         <v>82</v>
@@ -1679,6 +1679,41 @@
         <v>83</v>
       </c>
       <c r="K30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31">
+        <v>12166069</v>
+      </c>
+      <c r="F31">
+        <v>8603674</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aprimorei o visual HTML e CSS das páginas do App
</commit_message>
<xml_diff>
--- a/planilha/tarefas.xlsx
+++ b/planilha/tarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="93">
   <si>
     <t>Hoje</t>
   </si>
@@ -142,6 +142,15 @@
     <t>12/04/2023  10:38:24</t>
   </si>
   <si>
+    <t>12/04/2023  14:44:59</t>
+  </si>
+  <si>
+    <t>12/04/2023  15:02:14</t>
+  </si>
+  <si>
+    <t>12/04/2023  17:36:17</t>
+  </si>
+  <si>
     <t>YASMIN SANTOS PALHARES HORTA</t>
   </si>
   <si>
@@ -232,6 +241,15 @@
     <t>ELENICE DE SIQUEIRA</t>
   </si>
   <si>
+    <t>JENIFE BIANCA AMORIM PEREIRA</t>
+  </si>
+  <si>
+    <t>JUCIMAR AMORIM PEREIRA</t>
+  </si>
+  <si>
+    <t>VIRGILIO ISMAR SANTOS GARCIA</t>
+  </si>
+  <si>
     <t>1 dias úteis</t>
   </si>
   <si>
@@ -260,6 +278,9 @@
   </si>
   <si>
     <t>10 dias úteis</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
   <si>
     <t>NO</t>
@@ -629,7 +650,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -687,19 +708,19 @@
         <v>8577545</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -722,19 +743,19 @@
         <v>8578064</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -757,19 +778,19 @@
         <v>8579353</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -792,19 +813,19 @@
         <v>8580030</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="K5" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -827,19 +848,19 @@
         <v>8580119</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="K6" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -862,19 +883,19 @@
         <v>8580243</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -897,19 +918,19 @@
         <v>8580726</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -932,19 +953,19 @@
         <v>8230607</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -967,19 +988,19 @@
         <v>8581299</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1002,19 +1023,19 @@
         <v>8581975</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K11" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1037,19 +1058,19 @@
         <v>8583861</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K12" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1072,19 +1093,19 @@
         <v>8585862</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J13" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1107,19 +1128,19 @@
         <v>8586030</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I14" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K14" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1142,19 +1163,19 @@
         <v>8588077</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K15" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1177,19 +1198,19 @@
         <v>8588431</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J16" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K16" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1212,19 +1233,19 @@
         <v>8588645</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K17" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1247,19 +1268,19 @@
         <v>8589407</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J18" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K18" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1282,19 +1303,19 @@
         <v>8589813</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H19" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J19" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K19" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1317,19 +1338,19 @@
         <v>8591050</v>
       </c>
       <c r="G20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J20" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="K20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1352,19 +1373,19 @@
         <v>8591067</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J21" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1387,19 +1408,19 @@
         <v>8591079</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J22" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K22" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1422,19 +1443,19 @@
         <v>8591725</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I23" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J23" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K23" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1457,19 +1478,19 @@
         <v>8593801</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J24" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1492,19 +1513,19 @@
         <v>7797800</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J25" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K25" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1527,19 +1548,19 @@
         <v>8597675</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H26" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I26" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J26" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K26" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1562,19 +1583,19 @@
         <v>8598016</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H27" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I27" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K27" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1597,19 +1618,19 @@
         <v>8600473</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J28" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K28" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1632,19 +1653,19 @@
         <v>8601052</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I29" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J29" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K29" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1667,19 +1688,19 @@
         <v>8603359</v>
       </c>
       <c r="G30" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H30" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I30" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J30" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K30" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1702,19 +1723,124 @@
         <v>8603674</v>
       </c>
       <c r="G31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H31" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J31" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="K31" t="s">
-        <v>85</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32">
+        <v>12167081</v>
+      </c>
+      <c r="F32">
+        <v>8604741</v>
+      </c>
+      <c r="G32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" t="s">
+        <v>87</v>
+      </c>
+      <c r="I32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" t="s">
+        <v>90</v>
+      </c>
+      <c r="K32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33">
+        <v>12167165</v>
+      </c>
+      <c r="F33">
+        <v>8604741</v>
+      </c>
+      <c r="G33" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" t="s">
+        <v>87</v>
+      </c>
+      <c r="I33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J33" t="s">
+        <v>90</v>
+      </c>
+      <c r="K33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34">
+        <v>12167700</v>
+      </c>
+      <c r="F34">
+        <v>8605615</v>
+      </c>
+      <c r="G34" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" t="s">
+        <v>89</v>
+      </c>
+      <c r="J34" t="s">
+        <v>90</v>
+      </c>
+      <c r="K34" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
retrocedi melhorias e adaptei para notebook
</commit_message>
<xml_diff>
--- a/planilha/tarefas.xlsx
+++ b/planilha/tarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="95">
   <si>
     <t>Hoje</t>
   </si>
@@ -49,292 +49,211 @@
     <t>13-04-2023</t>
   </si>
   <si>
-    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
-  </si>
-  <si>
-    <t>29/03/2023  15:40:36</t>
-  </si>
-  <si>
-    <t>29/03/2023  17:18:47</t>
-  </si>
-  <si>
-    <t>30/03/2023  10:44:52</t>
-  </si>
-  <si>
-    <t>30/03/2023  14:42:51</t>
-  </si>
-  <si>
-    <t>30/03/2023  22:05:13</t>
-  </si>
-  <si>
-    <t>31/03/2023  09:33:21</t>
-  </si>
-  <si>
-    <t>31/03/2023  09:49:39</t>
-  </si>
-  <si>
-    <t>31/03/2023  11:43:24</t>
-  </si>
-  <si>
-    <t>01/04/2023  16:35:36</t>
-  </si>
-  <si>
-    <t>01/04/2023  16:55:34</t>
-  </si>
-  <si>
-    <t>03/04/2023  09:41:48</t>
-  </si>
-  <si>
-    <t>03/04/2023  14:02:31</t>
-  </si>
-  <si>
-    <t>03/04/2023  18:58:23</t>
-  </si>
-  <si>
-    <t>04/04/2023  09:27:21</t>
-  </si>
-  <si>
-    <t>04/04/2023  11:32:18</t>
-  </si>
-  <si>
-    <t>04/04/2023  14:57:51</t>
-  </si>
-  <si>
-    <t>04/04/2023  16:52:11</t>
-  </si>
-  <si>
-    <t>04/04/2023  17:48:58</t>
-  </si>
-  <si>
-    <t>05/04/2023  09:17:32</t>
-  </si>
-  <si>
-    <t>05/04/2023  09:38:27</t>
-  </si>
-  <si>
-    <t>05/04/2023  11:14:32</t>
-  </si>
-  <si>
-    <t>05/04/2023  14:58:01</t>
-  </si>
-  <si>
-    <t>05/04/2023  17:16:13</t>
-  </si>
-  <si>
-    <t>05/04/2023  18:37:46</t>
-  </si>
-  <si>
-    <t>06/04/2023  09:43:31</t>
-  </si>
-  <si>
-    <t>06/04/2023  17:07:51</t>
-  </si>
-  <si>
-    <t>10/04/2023  08:44:11</t>
-  </si>
-  <si>
-    <t>10/04/2023  11:56:29</t>
-  </si>
-  <si>
-    <t>10/04/2023  13:25:58</t>
-  </si>
-  <si>
-    <t>10/04/2023  14:54:09</t>
-  </si>
-  <si>
-    <t>10/04/2023  15:00:01</t>
-  </si>
-  <si>
-    <t>11/04/2023  08:23:00</t>
-  </si>
-  <si>
-    <t>11/04/2023  09:34:28</t>
-  </si>
-  <si>
-    <t>11/04/2023  13:50:53</t>
-  </si>
-  <si>
-    <t>11/04/2023  15:08:53</t>
-  </si>
-  <si>
-    <t>11/04/2023  16:57:02</t>
-  </si>
-  <si>
-    <t>12/04/2023  11:59:41</t>
-  </si>
-  <si>
-    <t>12/04/2023  12:03:08</t>
-  </si>
-  <si>
-    <t>12/04/2023  15:43:18</t>
-  </si>
-  <si>
-    <t>12/04/2023  16:14:52</t>
-  </si>
-  <si>
-    <t>13/04/2023  08:23:06</t>
-  </si>
-  <si>
-    <t>13/04/2023  11:42:27</t>
-  </si>
-  <si>
-    <t>13/04/2023  13:26:27</t>
-  </si>
-  <si>
-    <t>13/04/2023  15:12:39</t>
-  </si>
-  <si>
-    <t>13/04/2023  16:38:38</t>
-  </si>
-  <si>
-    <t>13/04/2023  16:46:57</t>
-  </si>
-  <si>
-    <t>13/04/2023  16:58:57</t>
-  </si>
-  <si>
-    <t>13/04/2023  18:17:42</t>
-  </si>
-  <si>
-    <t>MARILIA LUIZA OLIVEIRA DE MELO</t>
-  </si>
-  <si>
-    <t>LORRAYNE BALDI ANDRADE</t>
-  </si>
-  <si>
-    <t>MARIA CLAUDIA MENDES DA COSTA</t>
-  </si>
-  <si>
-    <t>ANDRESSA CASSANDRO STOFEL DE LIMA</t>
-  </si>
-  <si>
-    <t>FABIO DE VASCONCELOS MELO</t>
-  </si>
-  <si>
-    <t>ELIANE SANTOS XAVIER DAS NEVES</t>
-  </si>
-  <si>
-    <t>SUELI DOS SANTOS DA SILVA</t>
-  </si>
-  <si>
-    <t>MARCELINA CAMPELO DE SOUSA</t>
-  </si>
-  <si>
-    <t>SILMA MEDEIROS DO PATROCÃ­NIO</t>
-  </si>
-  <si>
-    <t>WERISLAYNI OLIVEIRA DA SILVA</t>
-  </si>
-  <si>
-    <t>RENATA ADRIANA DOS SANTOS NASCIMENTO</t>
-  </si>
-  <si>
-    <t>AUDILENE FERREIRA LOPES NASCIMENTO</t>
-  </si>
-  <si>
-    <t>ANDREZZA PEVAS DE ALMEIDA</t>
-  </si>
-  <si>
-    <t>MARIA CRISTINA TAVARES DA SILVA</t>
-  </si>
-  <si>
-    <t>ANA DRIELI DA SILVA LAGES</t>
-  </si>
-  <si>
-    <t>PYETRO SOUZA DE JESUS</t>
-  </si>
-  <si>
-    <t>MAURICEA DA SILVA CORREIA TAVARES</t>
-  </si>
-  <si>
-    <t>MARIA APARECIDA DA SILVA RIBEIRO</t>
-  </si>
-  <si>
-    <t>ALEXANDRE DE MELO WAGNER JUNIOR</t>
-  </si>
-  <si>
-    <t>SUELLEN PINHEIRO VIANA</t>
-  </si>
-  <si>
-    <t>EDNA LOPES DA SILVA</t>
-  </si>
-  <si>
-    <t>RHILLARY CAMILLE SOARES DE OLIVEIRA</t>
-  </si>
-  <si>
-    <t>SARAH DE OLIVEIRA PEREZ</t>
-  </si>
-  <si>
-    <t>CARLOS RODRIGO CHAGAS GITIRANA</t>
-  </si>
-  <si>
-    <t>CRISTIANO DE OLIVEIRA CARNEIRO</t>
-  </si>
-  <si>
-    <t>BRAYAN MIGUEL JAFFRA PEREIRA</t>
-  </si>
-  <si>
-    <t>JANAINA MARIA DA SILVA</t>
-  </si>
-  <si>
-    <t>CLEO DALSIOR VOM DOELINGER</t>
-  </si>
-  <si>
-    <t>WELLINGTON FERREIRA DE JESUS</t>
-  </si>
-  <si>
-    <t>BENICIO MARTINS FERNANDES</t>
-  </si>
-  <si>
-    <t>PAOLA MONIQUE DA SILVA TEIXEIRA</t>
-  </si>
-  <si>
-    <t>IDEILDO LUCENA MOURA DA SILVA JUNIOR</t>
-  </si>
-  <si>
-    <t>MARIA DA CONCEICAO DA SILVA</t>
-  </si>
-  <si>
-    <t>VALDIR FERNANDES DE ARAUJO</t>
-  </si>
-  <si>
-    <t>CALINE ESTEFANI DE SOUZA OLIVEIRA</t>
-  </si>
-  <si>
-    <t>MARLENE NUNES HONDA TAVARES</t>
-  </si>
-  <si>
-    <t>MARCO ANTONIO DALPRA</t>
-  </si>
-  <si>
-    <t>RAVI SCHULZ XAVIER DA CRUZ</t>
-  </si>
-  <si>
-    <t>KAYKY BRUNNO SOUZA LOPES</t>
-  </si>
-  <si>
-    <t>MÔNICA ALVES GOMES</t>
-  </si>
-  <si>
-    <t>MARCIO CANDIDO DE OLIVEIRA</t>
-  </si>
-  <si>
-    <t>BARBARA KELLY CARNEIRO LEÃO RODRIGUES</t>
-  </si>
-  <si>
-    <t>ANALIS SOARES SILVA</t>
-  </si>
-  <si>
-    <t>MAICKSON CAIQUE VENANCIO</t>
-  </si>
-  <si>
-    <t>EMILLE FERNANDES CORREA</t>
-  </si>
-  <si>
-    <t>MILENA FREIRE TRAVASSOS COUSSEIRO</t>
-  </si>
-  <si>
-    <t>ROGERIA DORALICE SOARES DA SILVA</t>
+    <t>417823 - PREMIUM SAÚDE S.A</t>
+  </si>
+  <si>
+    <t>29/03/2023  09:47:08</t>
+  </si>
+  <si>
+    <t>29/03/2023  12:30:46</t>
+  </si>
+  <si>
+    <t>29/03/2023  13:12:34</t>
+  </si>
+  <si>
+    <t>29/03/2023  13:31:59</t>
+  </si>
+  <si>
+    <t>29/03/2023  15:02:49</t>
+  </si>
+  <si>
+    <t>29/03/2023  16:41:58</t>
+  </si>
+  <si>
+    <t>29/03/2023  17:44:07</t>
+  </si>
+  <si>
+    <t>30/03/2023  10:18:35</t>
+  </si>
+  <si>
+    <t>30/03/2023  18:10:52</t>
+  </si>
+  <si>
+    <t>31/03/2023  15:44:32</t>
+  </si>
+  <si>
+    <t>31/03/2023  16:30:14</t>
+  </si>
+  <si>
+    <t>03/04/2023  13:44:27</t>
+  </si>
+  <si>
+    <t>03/04/2023  14:47:05</t>
+  </si>
+  <si>
+    <t>03/04/2023  15:25:17</t>
+  </si>
+  <si>
+    <t>03/04/2023  19:51:17</t>
+  </si>
+  <si>
+    <t>04/04/2023  09:49:35</t>
+  </si>
+  <si>
+    <t>04/04/2023  14:25:14</t>
+  </si>
+  <si>
+    <t>04/04/2023  14:37:21</t>
+  </si>
+  <si>
+    <t>04/04/2023  14:44:53</t>
+  </si>
+  <si>
+    <t>04/04/2023  16:42:14</t>
+  </si>
+  <si>
+    <t>05/04/2023  14:26:09</t>
+  </si>
+  <si>
+    <t>06/04/2023  13:03:51</t>
+  </si>
+  <si>
+    <t>10/04/2023  09:19:30</t>
+  </si>
+  <si>
+    <t>10/04/2023  10:47:50</t>
+  </si>
+  <si>
+    <t>11/04/2023  08:39:19</t>
+  </si>
+  <si>
+    <t>11/04/2023  11:09:14</t>
+  </si>
+  <si>
+    <t>12/04/2023  08:58:03</t>
+  </si>
+  <si>
+    <t>12/04/2023  10:38:24</t>
+  </si>
+  <si>
+    <t>12/04/2023  14:44:59</t>
+  </si>
+  <si>
+    <t>12/04/2023  15:02:14</t>
+  </si>
+  <si>
+    <t>12/04/2023  17:36:17</t>
+  </si>
+  <si>
+    <t>13/04/2023  10:06:53</t>
+  </si>
+  <si>
+    <t>13/04/2023  15:44:44</t>
+  </si>
+  <si>
+    <t>13/04/2023  17:09:35</t>
+  </si>
+  <si>
+    <t>GAEL AUGUSTO FERREIRA SANTOS</t>
+  </si>
+  <si>
+    <t>MARIANA FERREIRA BORGES</t>
+  </si>
+  <si>
+    <t>GILMAR DE JESUS</t>
+  </si>
+  <si>
+    <t>CLAUDETE APARECIDA SILVA</t>
+  </si>
+  <si>
+    <t>LARA EMANUELLY BARBOSA ALVES DE MELO</t>
+  </si>
+  <si>
+    <t>VALDIRA FOGACA FLORES</t>
+  </si>
+  <si>
+    <t>DURVALINA SOUZA PEREIRA</t>
+  </si>
+  <si>
+    <t>MARIA LENICE DA SILVA BOA VENTURA</t>
+  </si>
+  <si>
+    <t>PRISCILA TIZONI GOMES RIBEIRO SILVA</t>
+  </si>
+  <si>
+    <t>ALEXSANDRA RAMOS MARGARIDA</t>
+  </si>
+  <si>
+    <t>CREUZA CASTELLARI MARCONSINI REIS</t>
+  </si>
+  <si>
+    <t>BÁRBARA DE OLIVEIRA PATRÍCIO</t>
+  </si>
+  <si>
+    <t>KEPA FREDRICK STOCKNER</t>
+  </si>
+  <si>
+    <t>DAVIDSON LUIZ PEREIRA LOPES</t>
+  </si>
+  <si>
+    <t>KENIA CLAUDIA FARIA CAMPOS</t>
+  </si>
+  <si>
+    <t>CRISTIANE BATISTA ROCHA</t>
+  </si>
+  <si>
+    <t>ROBSON FRANCISCO LANZA JUNIOR</t>
+  </si>
+  <si>
+    <t>ANDREIA MARIA OTTONI MORAES</t>
+  </si>
+  <si>
+    <t>ANTONIA EVA MAGALHAES DOS SANTOS</t>
+  </si>
+  <si>
+    <t>ISIS NOGUEIRA CHAVES</t>
+  </si>
+  <si>
+    <t>ANTONIO CARLOS SANTOS</t>
+  </si>
+  <si>
+    <t>DANIELA FARIAS VASCONCELOS</t>
+  </si>
+  <si>
+    <t>CAIO HENRIQUE RODRIGUES FERNANDES</t>
+  </si>
+  <si>
+    <t>DIEGO SANTOS DE ALMEIDA</t>
+  </si>
+  <si>
+    <t>AYLA ALVES COELHO</t>
+  </si>
+  <si>
+    <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
+  </si>
+  <si>
+    <t>LUDIANE CONCEICAO DOS SANTOS OLIVEIRA MATOS</t>
+  </si>
+  <si>
+    <t>ELENICE DE SIQUEIRA</t>
+  </si>
+  <si>
+    <t>JENIFE BIANCA AMORIM PEREIRA</t>
+  </si>
+  <si>
+    <t>JUCIMAR AMORIM PEREIRA</t>
+  </si>
+  <si>
+    <t>VIRGILIO ISMAR SANTOS GARCIA</t>
+  </si>
+  <si>
+    <t>MELINDA GOULART CRUZ</t>
+  </si>
+  <si>
+    <t>JORGE EUSTACIO MEDEIROS</t>
+  </si>
+  <si>
+    <t>NATALIA SOLANO ROSSELIS PEREIRA DA SILVA</t>
   </si>
   <si>
     <t>1 dias úteis</t>
@@ -737,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -789,25 +708,25 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <v>12147299</v>
+        <v>12145988</v>
       </c>
       <c r="F2">
-        <v>8580883</v>
+        <v>8579353</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -824,25 +743,25 @@
         <v>13</v>
       </c>
       <c r="E3">
-        <v>12147571</v>
+        <v>12146576</v>
       </c>
       <c r="F3">
-        <v>8581252</v>
+        <v>8580030</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="J3" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="K3" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -859,25 +778,25 @@
         <v>14</v>
       </c>
       <c r="E4">
-        <v>12148282</v>
+        <v>12146711</v>
       </c>
       <c r="F4">
-        <v>8582107</v>
+        <v>8580119</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="J4" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="K4" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -894,25 +813,25 @@
         <v>15</v>
       </c>
       <c r="E5">
-        <v>12149112</v>
+        <v>12146787</v>
       </c>
       <c r="F5">
-        <v>8583135</v>
+        <v>8580243</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="I5" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="K5" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -929,25 +848,25 @@
         <v>16</v>
       </c>
       <c r="E6">
-        <v>12149924</v>
+        <v>12147152</v>
       </c>
       <c r="F6">
-        <v>8584156</v>
+        <v>8580726</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="J6" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="K6" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -964,25 +883,25 @@
         <v>17</v>
       </c>
       <c r="E7">
-        <v>12150089</v>
+        <v>12147478</v>
       </c>
       <c r="F7">
-        <v>8584343</v>
+        <v>8230607</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="J7" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K7" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -999,25 +918,25 @@
         <v>18</v>
       </c>
       <c r="E8">
-        <v>12150135</v>
+        <v>12147631</v>
       </c>
       <c r="F8">
-        <v>8584374</v>
+        <v>8581299</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="J8" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K8" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1034,25 +953,25 @@
         <v>19</v>
       </c>
       <c r="E9">
-        <v>12150483</v>
+        <v>12148200</v>
       </c>
       <c r="F9">
-        <v>8584813</v>
+        <v>8581975</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J9" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K9" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1069,25 +988,25 @@
         <v>20</v>
       </c>
       <c r="E10">
-        <v>12152006</v>
+        <v>12149727</v>
       </c>
       <c r="F10">
-        <v>8586692</v>
+        <v>8583861</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1104,25 +1023,25 @@
         <v>21</v>
       </c>
       <c r="E11">
-        <v>12152010</v>
+        <v>12151325</v>
       </c>
       <c r="F11">
-        <v>8586697</v>
+        <v>8585862</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="K11" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1139,25 +1058,25 @@
         <v>22</v>
       </c>
       <c r="E12">
-        <v>12152365</v>
+        <v>12151461</v>
       </c>
       <c r="F12">
-        <v>8587082</v>
+        <v>8586030</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J12" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K12" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1174,25 +1093,25 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>12153268</v>
+        <v>12153205</v>
       </c>
       <c r="F13">
-        <v>8588178</v>
+        <v>8588077</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J13" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K13" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1209,25 +1128,25 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>12154201</v>
+        <v>12153463</v>
       </c>
       <c r="F14">
-        <v>8589287</v>
+        <v>8588431</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J14" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1244,25 +1163,25 @@
         <v>25</v>
       </c>
       <c r="E15">
-        <v>12154563</v>
+        <v>12153630</v>
       </c>
       <c r="F15">
-        <v>8589717</v>
+        <v>8588645</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K15" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1279,25 +1198,25 @@
         <v>26</v>
       </c>
       <c r="E16">
-        <v>12154995</v>
+        <v>12154294</v>
       </c>
       <c r="F16">
-        <v>8590264</v>
+        <v>8589407</v>
       </c>
       <c r="G16" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J16" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K16" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1314,25 +1233,25 @@
         <v>27</v>
       </c>
       <c r="E17">
-        <v>12155773</v>
+        <v>12154631</v>
       </c>
       <c r="F17">
-        <v>8591144</v>
+        <v>8589813</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="H17" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="I17" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J17" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K17" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1349,25 +1268,25 @@
         <v>28</v>
       </c>
       <c r="E18">
-        <v>12156156</v>
+        <v>12155655</v>
       </c>
       <c r="F18">
-        <v>8591752</v>
+        <v>8591050</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="H18" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="I18" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J18" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="K18" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1384,25 +1303,25 @@
         <v>29</v>
       </c>
       <c r="E19">
-        <v>12156297</v>
+        <v>12155706</v>
       </c>
       <c r="F19">
-        <v>8591919</v>
+        <v>8591067</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J19" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K19" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1419,25 +1338,25 @@
         <v>30</v>
       </c>
       <c r="E20">
-        <v>12156771</v>
+        <v>12155732</v>
       </c>
       <c r="F20">
-        <v>8592489</v>
+        <v>8591079</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="I20" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J20" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K20" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1454,25 +1373,25 @@
         <v>31</v>
       </c>
       <c r="E21">
-        <v>12156826</v>
+        <v>12156130</v>
       </c>
       <c r="F21">
-        <v>8592529</v>
+        <v>8591725</v>
       </c>
       <c r="G21" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="H21" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J21" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K21" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1489,25 +1408,25 @@
         <v>32</v>
       </c>
       <c r="E22">
-        <v>12157160</v>
+        <v>12157899</v>
       </c>
       <c r="F22">
-        <v>8592956</v>
+        <v>8593801</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J22" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K22" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1524,25 +1443,25 @@
         <v>33</v>
       </c>
       <c r="E23">
-        <v>12158020</v>
+        <v>12159646</v>
       </c>
       <c r="F23">
-        <v>8593967</v>
+        <v>7797800</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H23" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="I23" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J23" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K23" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1559,25 +1478,25 @@
         <v>34</v>
       </c>
       <c r="E24">
-        <v>12158435</v>
+        <v>12161100</v>
       </c>
       <c r="F24">
-        <v>8594522</v>
+        <v>8597675</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H24" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="I24" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J24" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K24" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1594,25 +1513,25 @@
         <v>35</v>
       </c>
       <c r="E25">
-        <v>12158576</v>
+        <v>12161386</v>
       </c>
       <c r="F25">
-        <v>8594695</v>
+        <v>8598016</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="H25" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="I25" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J25" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K25" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1629,25 +1548,25 @@
         <v>36</v>
       </c>
       <c r="E26">
-        <v>12159014</v>
+        <v>12163407</v>
       </c>
       <c r="F26">
-        <v>8595238</v>
+        <v>8600473</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="H26" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="I26" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J26" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K26" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1664,25 +1583,25 @@
         <v>37</v>
       </c>
       <c r="E27">
-        <v>12160376</v>
+        <v>12163869</v>
       </c>
       <c r="F27">
-        <v>8596884</v>
+        <v>8601052</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="H27" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="I27" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J27" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K27" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1699,25 +1618,25 @@
         <v>38</v>
       </c>
       <c r="E28">
-        <v>12161017</v>
+        <v>12165805</v>
       </c>
       <c r="F28">
-        <v>8597595</v>
+        <v>8603359</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="I28" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J28" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="K28" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1734,25 +1653,25 @@
         <v>39</v>
       </c>
       <c r="E29">
-        <v>12161650</v>
+        <v>12166069</v>
       </c>
       <c r="F29">
-        <v>8598342</v>
+        <v>8603674</v>
       </c>
       <c r="G29" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="H29" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="I29" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J29" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="K29" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1769,25 +1688,25 @@
         <v>40</v>
       </c>
       <c r="E30">
-        <v>12162010</v>
+        <v>12167081</v>
       </c>
       <c r="F30">
-        <v>8598761</v>
+        <v>8604741</v>
       </c>
       <c r="G30" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H30" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="I30" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J30" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K30" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1804,25 +1723,25 @@
         <v>41</v>
       </c>
       <c r="E31">
-        <v>12162415</v>
+        <v>12167165</v>
       </c>
       <c r="F31">
-        <v>8599264</v>
+        <v>8604741</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="H31" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="I31" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J31" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K31" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1839,25 +1758,25 @@
         <v>42</v>
       </c>
       <c r="E32">
-        <v>12162439</v>
+        <v>12167700</v>
       </c>
       <c r="F32">
-        <v>8599230</v>
+        <v>8605615</v>
       </c>
       <c r="G32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H32" t="s">
         <v>89</v>
       </c>
-      <c r="H32" t="s">
-        <v>114</v>
-      </c>
       <c r="I32" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J32" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K32" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1874,25 +1793,25 @@
         <v>43</v>
       </c>
       <c r="E33">
-        <v>12163370</v>
+        <v>12168346</v>
       </c>
       <c r="F33">
-        <v>8600412</v>
+        <v>8606403</v>
       </c>
       <c r="G33" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="H33" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I33" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J33" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K33" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1909,25 +1828,25 @@
         <v>44</v>
       </c>
       <c r="E34">
-        <v>12163535</v>
+        <v>12169638</v>
       </c>
       <c r="F34">
-        <v>8600621</v>
+        <v>8608000</v>
       </c>
       <c r="G34" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="H34" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I34" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J34" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K34" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1944,515 +1863,25 @@
         <v>45</v>
       </c>
       <c r="E35">
-        <v>12164502</v>
+        <v>12169885</v>
       </c>
       <c r="F35">
-        <v>8601769</v>
+        <v>8608362</v>
       </c>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="H35" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="I35" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J35" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="K35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36">
-        <v>12164852</v>
-      </c>
-      <c r="F36">
-        <v>8602234</v>
-      </c>
-      <c r="G36" t="s">
-        <v>93</v>
-      </c>
-      <c r="H36" t="s">
-        <v>115</v>
-      </c>
-      <c r="I36" t="s">
-        <v>118</v>
-      </c>
-      <c r="J36" t="s">
-        <v>119</v>
-      </c>
-      <c r="K36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37">
-        <v>12165245</v>
-      </c>
-      <c r="F37">
-        <v>8602670</v>
-      </c>
-      <c r="G37" t="s">
-        <v>94</v>
-      </c>
-      <c r="H37" t="s">
-        <v>115</v>
-      </c>
-      <c r="I37" t="s">
-        <v>118</v>
-      </c>
-      <c r="J37" t="s">
-        <v>119</v>
-      </c>
-      <c r="K37" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38">
-        <v>12166383</v>
-      </c>
-      <c r="F38">
-        <v>8604036</v>
-      </c>
-      <c r="G38" t="s">
-        <v>95</v>
-      </c>
-      <c r="H38" t="s">
-        <v>116</v>
-      </c>
-      <c r="I38" t="s">
-        <v>118</v>
-      </c>
-      <c r="J38" t="s">
-        <v>119</v>
-      </c>
-      <c r="K38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39">
-        <v>12166396</v>
-      </c>
-      <c r="F39">
-        <v>8604069</v>
-      </c>
-      <c r="G39" t="s">
-        <v>96</v>
-      </c>
-      <c r="H39" t="s">
-        <v>116</v>
-      </c>
-      <c r="I39" t="s">
-        <v>118</v>
-      </c>
-      <c r="J39" t="s">
-        <v>119</v>
-      </c>
-      <c r="K39" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40">
-        <v>12167333</v>
-      </c>
-      <c r="F40">
-        <v>8605179</v>
-      </c>
-      <c r="G40" t="s">
-        <v>97</v>
-      </c>
-      <c r="H40" t="s">
-        <v>116</v>
-      </c>
-      <c r="I40" t="s">
-        <v>118</v>
-      </c>
-      <c r="J40" t="s">
-        <v>119</v>
-      </c>
-      <c r="K40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41">
-        <v>12167445</v>
-      </c>
-      <c r="F41">
-        <v>8605345</v>
-      </c>
-      <c r="G41" t="s">
-        <v>98</v>
-      </c>
-      <c r="H41" t="s">
-        <v>116</v>
-      </c>
-      <c r="I41" t="s">
-        <v>118</v>
-      </c>
-      <c r="J41" t="s">
-        <v>119</v>
-      </c>
-      <c r="K41" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" t="s">
-        <v>52</v>
-      </c>
-      <c r="E42">
-        <v>12168095</v>
-      </c>
-      <c r="F42">
-        <v>8606114</v>
-      </c>
-      <c r="G42" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" t="s">
-        <v>118</v>
-      </c>
-      <c r="J42" t="s">
-        <v>119</v>
-      </c>
-      <c r="K42" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43">
-        <v>12168687</v>
-      </c>
-      <c r="F43">
-        <v>8606848</v>
-      </c>
-      <c r="G43" t="s">
-        <v>100</v>
-      </c>
-      <c r="H43" t="s">
-        <v>116</v>
-      </c>
-      <c r="I43" t="s">
-        <v>118</v>
-      </c>
-      <c r="J43" t="s">
-        <v>119</v>
-      </c>
-      <c r="K43" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" t="s">
-        <v>54</v>
-      </c>
-      <c r="E44">
-        <v>12169086</v>
-      </c>
-      <c r="F44">
-        <v>8607367</v>
-      </c>
-      <c r="G44" t="s">
-        <v>101</v>
-      </c>
-      <c r="H44" t="s">
-        <v>116</v>
-      </c>
-      <c r="I44" t="s">
-        <v>118</v>
-      </c>
-      <c r="J44" t="s">
-        <v>119</v>
-      </c>
-      <c r="K44" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" t="s">
-        <v>55</v>
-      </c>
-      <c r="E45">
-        <v>12169516</v>
-      </c>
-      <c r="F45">
-        <v>8607900</v>
-      </c>
-      <c r="G45" t="s">
-        <v>102</v>
-      </c>
-      <c r="H45" t="s">
-        <v>116</v>
-      </c>
-      <c r="I45" t="s">
-        <v>118</v>
-      </c>
-      <c r="J45" t="s">
-        <v>119</v>
-      </c>
-      <c r="K45" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46">
-        <v>12169806</v>
-      </c>
-      <c r="F46">
-        <v>8608265</v>
-      </c>
-      <c r="G46" t="s">
-        <v>103</v>
-      </c>
-      <c r="H46" t="s">
-        <v>116</v>
-      </c>
-      <c r="I46" t="s">
-        <v>118</v>
-      </c>
-      <c r="J46" t="s">
-        <v>119</v>
-      </c>
-      <c r="K46" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="1">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47">
-        <v>12169830</v>
-      </c>
-      <c r="F47">
-        <v>8608288</v>
-      </c>
-      <c r="G47" t="s">
-        <v>104</v>
-      </c>
-      <c r="H47" t="s">
-        <v>116</v>
-      </c>
-      <c r="I47" t="s">
-        <v>118</v>
-      </c>
-      <c r="J47" t="s">
-        <v>119</v>
-      </c>
-      <c r="K47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" t="s">
-        <v>58</v>
-      </c>
-      <c r="E48">
-        <v>12169862</v>
-      </c>
-      <c r="F48">
-        <v>8608371</v>
-      </c>
-      <c r="G48" t="s">
-        <v>105</v>
-      </c>
-      <c r="H48" t="s">
-        <v>116</v>
-      </c>
-      <c r="I48" t="s">
-        <v>118</v>
-      </c>
-      <c r="J48" t="s">
-        <v>119</v>
-      </c>
-      <c r="K48" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="1">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" t="s">
-        <v>59</v>
-      </c>
-      <c r="E49">
-        <v>12170051</v>
-      </c>
-      <c r="F49">
-        <v>8608573</v>
-      </c>
-      <c r="G49" t="s">
-        <v>106</v>
-      </c>
-      <c r="H49" t="s">
-        <v>116</v>
-      </c>
-      <c r="I49" t="s">
-        <v>118</v>
-      </c>
-      <c r="J49" t="s">
-        <v>119</v>
-      </c>
-      <c r="K49" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit depois do erro Word
</commit_message>
<xml_diff>
--- a/planilha/tarefas.xlsx
+++ b/planilha/tarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="160">
   <si>
     <t>Operadora</t>
   </si>
@@ -64,7 +64,7 @@
     <t>18-04-2023</t>
   </si>
   <si>
-    <t>Extraï¿½do em 18/04/2023 15:43</t>
+    <t>Extraï¿½do em 18/04/2023 18:07</t>
   </si>
   <si>
     <t>Sistema Integrado de Fiscalizaï¿½ï¿½o - NIP</t>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Interlocutora, que se identifica como mãe do beneficiário, questiona a falta de atendimento para TERAPIA OCUPACIONAL, FONOAUDIOLOGO E PSICOLOGO. A solicitação foi feita à Operadora em Janeiro/2023, para realização no município Belo Horizonte/MG. A operadora não apresenta resposta ao pedido. Protocolo: 34852020230418853930 Data: 18/04/2023.</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
   <si>
     <t>NO</t>
@@ -1058,7 +1061,7 @@
         <v>156</v>
       </c>
       <c r="L9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1096,7 +1099,7 @@
         <v>156</v>
       </c>
       <c r="L10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1134,7 +1137,7 @@
         <v>156</v>
       </c>
       <c r="L11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1172,7 +1175,7 @@
         <v>156</v>
       </c>
       <c r="L12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1207,10 +1210,10 @@
         <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1245,10 +1248,10 @@
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1283,10 +1286,10 @@
         <v>2</v>
       </c>
       <c r="K15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1321,10 +1324,10 @@
         <v>2</v>
       </c>
       <c r="K16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1359,10 +1362,10 @@
         <v>2</v>
       </c>
       <c r="K17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1397,10 +1400,10 @@
         <v>3</v>
       </c>
       <c r="K18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1435,10 +1438,10 @@
         <v>4</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1473,10 +1476,10 @@
         <v>5</v>
       </c>
       <c r="K20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1511,10 +1514,10 @@
         <v>5</v>
       </c>
       <c r="K21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1549,10 +1552,10 @@
         <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1587,10 +1590,10 @@
         <v>6</v>
       </c>
       <c r="K23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1625,10 +1628,10 @@
         <v>7</v>
       </c>
       <c r="K24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1663,10 +1666,10 @@
         <v>7</v>
       </c>
       <c r="K25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1701,10 +1704,10 @@
         <v>7</v>
       </c>
       <c r="K26" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L26" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1739,10 +1742,10 @@
         <v>7</v>
       </c>
       <c r="K27" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1777,10 +1780,10 @@
         <v>7</v>
       </c>
       <c r="K28" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1815,10 +1818,10 @@
         <v>8</v>
       </c>
       <c r="K29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L29" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1853,10 +1856,10 @@
         <v>8</v>
       </c>
       <c r="K30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1891,10 +1894,10 @@
         <v>8</v>
       </c>
       <c r="K31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1929,10 +1932,10 @@
         <v>9</v>
       </c>
       <c r="K32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L32" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1967,10 +1970,10 @@
         <v>9</v>
       </c>
       <c r="K33" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2002,10 +2005,10 @@
         <v>9</v>
       </c>
       <c r="K34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2040,10 +2043,10 @@
         <v>10</v>
       </c>
       <c r="K35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L35" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2078,10 +2081,10 @@
         <v>10</v>
       </c>
       <c r="K36" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2116,10 +2119,10 @@
         <v>10</v>
       </c>
       <c r="K37" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2154,10 +2157,10 @@
         <v>10</v>
       </c>
       <c r="K38" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2192,10 +2195,10 @@
         <v>10</v>
       </c>
       <c r="K39" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L39" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2230,10 +2233,10 @@
         <v>10</v>
       </c>
       <c r="K40" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L40" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2268,10 +2271,10 @@
         <v>10</v>
       </c>
       <c r="K41" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L41" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2306,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="K42" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L42" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>